<commit_message>
[MDTUDDM-25344] Updated registry min template pricing
Change-Id: I8165e7edf7286f3094af795cfd9c4abb170ccd54
</commit_message>
<xml_diff>
--- a/modules/arch/attachments/architecture/registry_cost_calculator.xlsx
+++ b/modules/arch/attachments/architecture/registry_cost_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton_Tupitsyn\work\MTDU-DDM\gerrit\ddm-architecture\modules\arch\attachments\architecture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/modules/arch/attachments/architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C0728D-E1FD-420B-9EE8-74709073150D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2010A9C8-56D1-2949-9918-387D581D567A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{27F18D04-7E62-4946-83A8-E11013D50C84}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{27F18D04-7E62-4946-83A8-E11013D50C84}"/>
   </bookViews>
   <sheets>
     <sheet name="Калькулятор вартості" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="109">
   <si>
     <t>Всього робочих годин в місяць</t>
   </si>
@@ -362,13 +362,16 @@
   </si>
   <si>
     <t>&gt;100000</t>
+  </si>
+  <si>
+    <t>1 VM calculation reference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -459,6 +462,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -542,14 +546,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -619,6 +620,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,100 +938,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2669E3AB-101C-8547-83F4-DF3AE92242F5}">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.09765625" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.09765625" customWidth="1"/>
-    <col min="4" max="4" width="11.8984375" customWidth="1"/>
-    <col min="5" max="5" width="8.59765625" customWidth="1"/>
-    <col min="6" max="6" width="9.09765625" customWidth="1"/>
-    <col min="7" max="7" width="10.09765625" customWidth="1"/>
-    <col min="8" max="8" width="10.59765625" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="11.8984375" customWidth="1"/>
-    <col min="11" max="11" width="8.59765625" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="14" max="18" width="12.09765625" customWidth="1"/>
-    <col min="20" max="20" width="13.09765625" customWidth="1"/>
+    <col min="14" max="18" width="12.1640625" customWidth="1"/>
+    <col min="20" max="20" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="9"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="9" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <f>30*24</f>
         <v>720</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="19">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="18">
         <f>5*4*12</f>
         <v>240</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20"/>
+      <c r="D3" s="19"/>
       <c r="E3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>80</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-    </row>
-    <row r="7" spans="1:22" ht="78">
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+    </row>
+    <row r="7" spans="1:22" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1090,547 +1095,626 @@
       <c r="U7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V7" s="15" t="s">
+      <c r="V7" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:22" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C8" s="31">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10">
         <v>0.46</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="31">
         <f>C8*D8</f>
         <v>0.46</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="31">
         <v>120</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="I8" s="3">
-        <f>G8*H8</f>
+      <c r="I8" s="31">
+        <f>G8*H8*C8</f>
         <v>11.424000000000001</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="31">
         <v>200</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="11">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="31">
         <f>K8*L8</f>
         <v>19.040000000000003</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="31">
         <v>550</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="31">
         <f>IF(N8&lt;=10000, 0.09 * N8, 10000*0.09)</f>
         <v>49.5</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="31">
         <f>IF(N8&gt;10000, IF(N8&lt;=50000, 0.085 * (N8-10000), 40000*0.085), 0)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="31">
         <f>IF(O8&gt;50000,IF(O8&lt;=150000,0.07*(O8-50000),100000*0.07),0)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="31">
         <f>IF(N8&gt;150000,(N8-150000)*0.05,0)</f>
         <v>0</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8" s="31">
         <f>SUM(O8:R8)</f>
         <v>49.5</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="31">
         <f>$B$3*E8+I8+M8+S8</f>
         <v>190.364</v>
       </c>
-      <c r="U8" s="3">
-        <f>J$23/$B$4*C8</f>
+      <c r="U8" s="31">
+        <f>J$24/$B$4*C8</f>
         <v>129.26185000000001</v>
       </c>
-      <c r="V8" s="16">
+      <c r="V8" s="15">
         <f>T8+U8</f>
         <v>319.62585000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:22" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="3">
-        <v>5</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C9" s="31">
+        <v>2</v>
+      </c>
+      <c r="D9" s="10">
         <v>0.46</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="31">
         <f>C9*D9</f>
-        <v>2.3000000000000003</v>
-      </c>
-      <c r="F9" s="3" t="s">
+        <v>0.92</v>
+      </c>
+      <c r="F9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="31">
         <v>120</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="31">
         <f>G9*H9*C9</f>
-        <v>57.120000000000005</v>
-      </c>
-      <c r="J9" s="3" t="s">
+        <v>22.848000000000003</v>
+      </c>
+      <c r="J9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="31">
         <v>200</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="11">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="31">
         <f>K9*L9</f>
         <v>19.040000000000003</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="31">
         <v>550</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="31">
         <f>IF(N9&lt;=10000, 0.09 * N9, 10000*0.09)</f>
         <v>49.5</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="31">
         <f>IF(N9&gt;10000, IF(N9&lt;=50000, 0.085 * (N9-10000), 40000*0.085), 0)</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="3">
-        <f>IF(N9&gt;50000,IF(N9&lt;=150000,0.07*(N9-50000),100000*0.07),0)</f>
+      <c r="Q9" s="31">
+        <f>IF(O9&gt;50000,IF(O9&lt;=150000,0.07*(O9-50000),100000*0.07),0)</f>
         <v>0</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="31">
         <f>IF(N9&gt;150000,(N9-150000)*0.05,0)</f>
         <v>0</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="31">
         <f>SUM(O9:R9)</f>
         <v>49.5</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="31">
         <f>$B$3*E9+I9+M9+S9</f>
-        <v>677.66000000000008</v>
-      </c>
-      <c r="U9" s="3">
-        <f>J$23/$B$4*C9</f>
-        <v>646.30925000000002</v>
-      </c>
-      <c r="V9" s="16">
-        <f t="shared" ref="V9:V10" si="0">T9+U9</f>
-        <v>1323.9692500000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="10" t="s">
+        <v>312.18800000000005</v>
+      </c>
+      <c r="U9" s="31">
+        <f>J$24/$B$4*C9</f>
+        <v>258.52370000000002</v>
+      </c>
+      <c r="V9" s="15">
+        <f>T9+U9</f>
+        <v>570.71170000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="3">
-        <v>10</v>
-      </c>
-      <c r="D10" s="11">
+      <c r="C10" s="31">
+        <v>5</v>
+      </c>
+      <c r="D10" s="10">
         <v>0.46</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="31">
         <f>C10*D10</f>
-        <v>4.6000000000000005</v>
-      </c>
-      <c r="F10" s="3" t="s">
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="F10" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="31">
         <v>120</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="11">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="31">
         <f>G10*H10*C10</f>
-        <v>114.24000000000001</v>
-      </c>
-      <c r="J10" s="3" t="s">
+        <v>57.120000000000005</v>
+      </c>
+      <c r="J10" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="31">
         <v>200</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="11">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="31">
         <f>K10*L10</f>
         <v>19.040000000000003</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="31">
         <v>550</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="31">
         <f>IF(N10&lt;=10000, 0.09 * N10, 10000*0.09)</f>
         <v>49.5</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="31">
         <f>IF(N10&gt;10000, IF(N10&lt;=50000, 0.085 * (N10-10000), 40000*0.085), 0)</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="3">
-        <f>IF(O10&gt;50000,IF(O10&lt;=150000,0.07*(O10-50000),100000*0.07),0)</f>
+      <c r="Q10" s="31">
+        <f>IF(N10&gt;50000,IF(N10&lt;=150000,0.07*(N10-50000),100000*0.07),0)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10" s="31">
         <f>IF(N10&gt;150000,(N10-150000)*0.05,0)</f>
         <v>0</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10" s="31">
         <f>SUM(O10:R10)</f>
         <v>49.5</v>
       </c>
-      <c r="T10" s="3">
-        <f t="shared" ref="T10" si="1">$B$3*E10+I10+M10+S10</f>
+      <c r="T10" s="31">
+        <f>$B$3*E10+I10+M10+S10</f>
+        <v>677.66000000000008</v>
+      </c>
+      <c r="U10" s="31">
+        <f>J$24/$B$4*C10</f>
+        <v>646.30925000000002</v>
+      </c>
+      <c r="V10" s="15">
+        <f t="shared" ref="V10:V11" si="0">T10+U10</f>
+        <v>1323.9692500000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="31">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.46</v>
+      </c>
+      <c r="E11" s="31">
+        <f>C11*D11</f>
+        <v>4.6000000000000005</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="31">
+        <v>120</v>
+      </c>
+      <c r="H11" s="11">
+        <v>9.5200000000000007E-2</v>
+      </c>
+      <c r="I11" s="31">
+        <f>G11*H11*C11</f>
+        <v>114.24000000000001</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="31">
+        <v>200</v>
+      </c>
+      <c r="L11" s="11">
+        <v>9.5200000000000007E-2</v>
+      </c>
+      <c r="M11" s="31">
+        <f>K11*L11</f>
+        <v>19.040000000000003</v>
+      </c>
+      <c r="N11" s="31">
+        <v>550</v>
+      </c>
+      <c r="O11" s="31">
+        <f>IF(N11&lt;=10000, 0.09 * N11, 10000*0.09)</f>
+        <v>49.5</v>
+      </c>
+      <c r="P11" s="31">
+        <f>IF(N11&gt;10000, IF(N11&lt;=50000, 0.085 * (N11-10000), 40000*0.085), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="31">
+        <f>IF(O11&gt;50000,IF(O11&lt;=150000,0.07*(O11-50000),100000*0.07),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="31">
+        <f>IF(N11&gt;150000,(N11-150000)*0.05,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="31">
+        <f>SUM(O11:R11)</f>
+        <v>49.5</v>
+      </c>
+      <c r="T11" s="31">
+        <f t="shared" ref="T11" si="1">$B$3*E11+I11+M11+S11</f>
         <v>1286.7800000000002</v>
       </c>
-      <c r="U10" s="3">
-        <f t="shared" ref="U10" si="2">J$23/$B$4*C10</f>
+      <c r="U11" s="31">
+        <f t="shared" ref="U11" si="2">J$24/$B$4*C11</f>
         <v>1292.6185</v>
       </c>
-      <c r="V10" s="16">
+      <c r="V11" s="15">
         <f t="shared" si="0"/>
         <v>2579.3985000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="31" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-    </row>
-    <row r="15" spans="1:22" ht="93.6">
-      <c r="A15" s="14" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+    </row>
+    <row r="16" spans="1:22" ht="102" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J16" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C17" s="3">
         <v>3</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D17" s="3">
         <v>0.60799999999999998</v>
       </c>
-      <c r="E16" s="4">
-        <f t="shared" ref="E16:E22" si="3">C16*D16</f>
+      <c r="E17" s="3">
+        <f t="shared" ref="E17:E23" si="3">C17*D17</f>
         <v>1.8239999999999998</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G17" s="3">
         <v>120</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H17" s="5">
         <v>0.11899999999999999</v>
       </c>
-      <c r="I16" s="4">
-        <f t="shared" ref="I16:I22" si="4">G16*H16*C16</f>
+      <c r="I17" s="3">
+        <f t="shared" ref="I17:I23" si="4">G17*H17*C17</f>
         <v>42.839999999999996</v>
       </c>
-      <c r="J16" s="4">
-        <f>B$2*E16+I16</f>
+      <c r="J17" s="3">
+        <f>B$2*E17+I17</f>
         <v>1356.12</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C18" s="3">
         <v>3</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D18" s="4">
         <v>1.216</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E18" s="3">
         <f t="shared" si="3"/>
         <v>3.6479999999999997</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G18" s="6">
         <f>1000+120+50</f>
         <v>1170</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H18" s="5">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I18" s="3">
         <f t="shared" si="4"/>
         <v>334.15200000000004</v>
       </c>
-      <c r="J17" s="4">
-        <f t="shared" ref="J17:J22" si="5">B$2*E17+I17</f>
+      <c r="J18" s="3">
+        <f t="shared" ref="J18:J23" si="5">B$2*E18+I18</f>
         <v>2960.712</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D19" s="7">
         <v>0.46</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E19" s="3">
         <f t="shared" si="3"/>
         <v>1.3800000000000001</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G19" s="3">
         <f>375+120</f>
         <v>495</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H19" s="5">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I19" s="3">
         <f t="shared" si="4"/>
         <v>141.37200000000001</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J19" s="3">
         <f t="shared" si="5"/>
         <v>1134.9720000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C20" s="3">
         <v>5</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D20" s="3">
         <v>0.60799999999999998</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E20" s="3">
         <f t="shared" si="3"/>
         <v>3.04</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G20" s="3">
         <f>120+(100+400+100+50)/5</f>
         <v>250</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H20" s="3">
         <v>0.11899999999999999</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I20" s="27">
         <f t="shared" si="4"/>
         <v>148.75</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J20" s="3">
         <f t="shared" si="5"/>
         <v>2337.5500000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="22" customFormat="1">
-      <c r="A20" s="21" t="s">
+    <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="21">
-        <v>1</v>
-      </c>
-      <c r="D20" s="21">
+      <c r="C21" s="20">
+        <v>1</v>
+      </c>
+      <c r="D21" s="20">
         <v>0.60799999999999998</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E21" s="20">
         <f t="shared" si="3"/>
         <v>0.60799999999999998</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F21" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G21" s="20">
         <v>160</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H21" s="20">
         <v>0.11899999999999999</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I21" s="27">
         <f t="shared" si="4"/>
         <v>19.04</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J21" s="3">
         <f t="shared" si="5"/>
         <v>456.8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="22" customFormat="1">
-      <c r="A21" s="21" t="s">
+    <row r="22" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="21">
-        <v>1</v>
-      </c>
-      <c r="D21" s="21">
+      <c r="C22" s="20">
+        <v>1</v>
+      </c>
+      <c r="D22" s="20">
         <v>0.60799999999999998</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E22" s="20">
         <f t="shared" si="3"/>
         <v>0.60799999999999998</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F22" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G22" s="20">
         <v>2080</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H22" s="20">
         <v>0.11899999999999999</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I22" s="27">
         <f t="shared" si="4"/>
         <v>247.51999999999998</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J22" s="3">
         <f t="shared" si="5"/>
         <v>685.28</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="22" customFormat="1">
-      <c r="A22" s="21" t="s">
+    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="21">
-        <v>1</v>
-      </c>
-      <c r="D22" s="21">
+      <c r="C23" s="20">
+        <v>1</v>
+      </c>
+      <c r="D23" s="20">
         <v>0.60799999999999998</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E23" s="20">
         <f t="shared" si="3"/>
         <v>0.60799999999999998</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F23" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G23" s="20">
         <v>160</v>
       </c>
-      <c r="H22" s="21">
+      <c r="H23" s="20">
         <v>0.11899999999999999</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I23" s="27">
         <f t="shared" si="4"/>
         <v>19.04</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J23" s="3">
         <f t="shared" si="5"/>
         <v>456.8</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="I23" s="17" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I24" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="J23" s="16">
-        <f>SUM(J16:J22)+SUM(I16:I22)</f>
+      <c r="J24" s="15">
+        <f>SUM(J17:J23)+SUM(I17:I23)</f>
         <v>10340.948</v>
       </c>
     </row>
@@ -1638,10 +1722,11 @@
   <mergeCells count="3">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A6:V6"/>
-    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A15:J15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1650,65 +1735,64 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.59765625" customWidth="1"/>
-    <col min="2" max="3" width="15.09765625" customWidth="1"/>
-    <col min="4" max="4" width="14.59765625" customWidth="1"/>
-    <col min="6" max="6" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="49.6640625" customWidth="1"/>
+    <col min="2" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
       <c r="B2">
         <f>CEILING(MAX(C5,C10:C12,C24:G24), 1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <f>B2*C6*720*'Калькулятор вартості'!E8+B2*'Калькулятор вартості'!I8+'Калькулятор вартості'!M8+'Калькулятор вартості'!S8+B2*'Калькулятор вартості'!U8</f>
-        <v>319.62585000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="F3" s="22"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="23" t="s">
+        <v>570.71170000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>Словники!A1</f>
         <v>Режим високої доступності</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="C5">
-        <f>VLOOKUP(B5,Словники!A2:B3,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="1:7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>Словники!C1</f>
         <v>Режим роботи</v>
@@ -1716,20 +1800,20 @@
       <c r="B6" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="25">
         <f>VLOOKUP(B6,Словники!C2:D4,2,FALSE)</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>Словники!A6</f>
         <v>Кількість бізнес сутностей</v>
@@ -1742,7 +1826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>Словники!C6</f>
         <v>Максимальна кількість екземплярів бізнес сутностей (рядків в таблиці)</v>
@@ -1755,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>Словники!E6</f>
         <v>Приблизний об'єм історичних даних в GB</v>
@@ -1768,30 +1852,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="23" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>Словники!A12</f>
         <v>Кількість користувачів</v>
@@ -1818,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>Словники!C12</f>
         <v>Кількість послуг (бізнес-процесів)</v>
@@ -1845,7 +1929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>Словники!E12</f>
         <v>Середня кількість задач для користувачів на послугу</v>
@@ -1864,10 +1948,10 @@
         <f>VLOOKUP(D19,Словники!$E$19:'Словники'!$F$21,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>Словники!G12</f>
         <v>Середня кількість автоматизованих задач на послугу</v>
@@ -1894,7 +1978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>Словники!I12</f>
         <v>Кількість звітів</v>
@@ -1906,12 +1990,12 @@
         <f>VLOOKUP(B21,Словники!$I$13:'Словники'!$J$15,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>Словники!K12</f>
         <v>Кількість витягів</v>
@@ -1938,13 +2022,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>Словники!M12</f>
         <v>Кількість надаваємих послуг в місяць</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" t="s">
         <v>98</v>
       </c>
@@ -1960,8 +2044,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="22"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="21"/>
       <c r="C24">
         <f>MAX(C17:C23)</f>
         <v>1</v>
@@ -2141,35 +2225,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C2CE02-549B-42BB-BB2B-79BD8E0A657F}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.59765625" customWidth="1"/>
-    <col min="2" max="2" width="15.8984375" customWidth="1"/>
-    <col min="3" max="3" width="42.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.59765625" customWidth="1"/>
-    <col min="7" max="7" width="44.09765625" customWidth="1"/>
-    <col min="9" max="9" width="15.59765625" customWidth="1"/>
-    <col min="11" max="11" width="23.8984375" customWidth="1"/>
-    <col min="13" max="13" width="39.59765625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="7" max="7" width="44.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" customWidth="1"/>
+    <col min="13" max="13" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
         <v>83</v>
       </c>
       <c r="B1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>84</v>
       </c>
       <c r="D1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -2183,22 +2269,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <f>240/720</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>54</v>
       </c>
@@ -2206,27 +2292,27 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
         <v>85</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>86</v>
       </c>
       <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>87</v>
       </c>
       <c r="F6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2246,27 +2332,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
         <v>67</v>
       </c>
       <c r="B8">
         <v>1.2</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>78</v>
       </c>
       <c r="D8">
         <v>1.2</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>79</v>
       </c>
       <c r="F8">
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -2286,56 +2372,56 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="23" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>90</v>
       </c>
       <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>91</v>
       </c>
       <c r="F12" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="22" t="s">
         <v>92</v>
       </c>
       <c r="H12" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="22" t="s">
         <v>93</v>
       </c>
       <c r="J12" t="s">
         <v>52</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="22" t="s">
         <v>94</v>
       </c>
       <c r="L12" t="s">
         <v>52</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="22" t="s">
         <v>95</v>
       </c>
       <c r="N12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -2373,45 +2459,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
         <v>64</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>67</v>
       </c>
       <c r="D14">
         <v>1.5</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>81</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="24" t="s">
         <v>71</v>
       </c>
       <c r="H14">
         <v>2</v>
       </c>
-      <c r="I14" s="25" t="s">
+      <c r="I14" s="24" t="s">
         <v>67</v>
       </c>
       <c r="J14">
         <v>1.5</v>
       </c>
-      <c r="K14" s="25" t="s">
+      <c r="K14" s="24" t="s">
         <v>67</v>
       </c>
       <c r="L14">
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -2449,56 +2535,56 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="23" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="23" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B18" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>90</v>
       </c>
       <c r="D18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="22" t="s">
         <v>91</v>
       </c>
       <c r="F18" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="22" t="s">
         <v>92</v>
       </c>
       <c r="H18" t="s">
         <v>52</v>
       </c>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="22" t="s">
         <v>93</v>
       </c>
       <c r="J18" t="s">
         <v>52</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="22" t="s">
         <v>94</v>
       </c>
       <c r="L18" t="s">
         <v>52</v>
       </c>
-      <c r="M18" s="23" t="s">
+      <c r="M18" s="22" t="s">
         <v>95</v>
       </c>
       <c r="N18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -2536,46 +2622,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="25" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
         <v>99</v>
       </c>
       <c r="B20">
         <v>5</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="24" t="s">
         <v>67</v>
       </c>
       <c r="D20">
         <v>1.5</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="24" t="s">
         <v>69</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="24" t="s">
         <v>71</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
-      <c r="I20" s="25"/>
-      <c r="K20" s="25" t="s">
+      <c r="I20" s="24"/>
+      <c r="K20" s="24" t="s">
         <v>67</v>
       </c>
       <c r="L20">
         <v>1.5</v>
       </c>
-      <c r="M20" s="25" t="s">
+      <c r="M20" s="24" t="s">
         <v>73</v>
       </c>
       <c r="N20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -2613,56 +2699,56 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B24" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="22" t="s">
         <v>90</v>
       </c>
       <c r="D24" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="22" t="s">
         <v>91</v>
       </c>
       <c r="F24" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="22" t="s">
         <v>92</v>
       </c>
       <c r="H24" t="s">
         <v>52</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="22" t="s">
         <v>93</v>
       </c>
       <c r="J24" t="s">
         <v>52</v>
       </c>
-      <c r="K24" s="23" t="s">
+      <c r="K24" s="22" t="s">
         <v>94</v>
       </c>
       <c r="L24" t="s">
         <v>52</v>
       </c>
-      <c r="M24" s="23" t="s">
+      <c r="M24" s="22" t="s">
         <v>95</v>
       </c>
       <c r="N24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -2700,46 +2786,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="25" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="24" t="s">
         <v>103</v>
       </c>
       <c r="B26">
         <v>5</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="24" t="s">
         <v>104</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="G26" s="25" t="s">
+      <c r="E26" s="24"/>
+      <c r="G26" s="24" t="s">
         <v>71</v>
       </c>
       <c r="H26">
         <v>2</v>
       </c>
-      <c r="I26" s="25" t="s">
+      <c r="I26" s="24" t="s">
         <v>67</v>
       </c>
       <c r="J26">
         <v>1.5</v>
       </c>
-      <c r="K26" s="25" t="s">
+      <c r="K26" s="24" t="s">
         <v>67</v>
       </c>
       <c r="L26">
         <v>2</v>
       </c>
-      <c r="M26" s="25" t="s">
+      <c r="M26" s="24" t="s">
         <v>105</v>
       </c>
       <c r="N26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2784,6 +2870,40 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="346a80a9-3278-4844-b436-58ae57568790">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a2d094e0-efa8-4820-a0b3-29af30f3c512" xsi:nil="true"/>
+    <SharedWithUsers xmlns="a2d094e0-efa8-4820-a0b3-29af30f3c512">
+      <UserInfo>
+        <DisplayName>Vitalii Fedorenko</DisplayName>
+        <AccountId>158</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Oleksandr Zakusylo</DisplayName>
+        <AccountId>159</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <Capability_x0020_name xmlns="346a80a9-3278-4844-b436-58ae57568790"/>
+    <Release xmlns="346a80a9-3278-4844-b436-58ae57568790" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010022314AB35D24274D94E93A0CCD2DBC5F" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3febe1d67782b5c77e50c43cf0e433a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="346a80a9-3278-4844-b436-58ae57568790" xmlns:ns3="a2d094e0-efa8-4820-a0b3-29af30f3c512" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a828650ea744d4614f15fd37c541cd95" ns2:_="" ns3:_="">
     <xsd:import namespace="346a80a9-3278-4844-b436-58ae57568790"/>
@@ -3042,41 +3162,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD363066-8CBD-4D6F-8835-7EB8A1E12EC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="346a80a9-3278-4844-b436-58ae57568790"/>
+    <ds:schemaRef ds:uri="a2d094e0-efa8-4820-a0b3-29af30f3c512"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="346a80a9-3278-4844-b436-58ae57568790">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a2d094e0-efa8-4820-a0b3-29af30f3c512" xsi:nil="true"/>
-    <SharedWithUsers xmlns="a2d094e0-efa8-4820-a0b3-29af30f3c512">
-      <UserInfo>
-        <DisplayName>Vitalii Fedorenko</DisplayName>
-        <AccountId>158</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Oleksandr Zakusylo</DisplayName>
-        <AccountId>159</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <Capability_x0020_name xmlns="346a80a9-3278-4844-b436-58ae57568790"/>
-    <Release xmlns="346a80a9-3278-4844-b436-58ae57568790" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92FEC7CF-4815-42BA-A053-9D2F9AB7FD60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D39A1E4B-89AB-4EF2-84C8-5084CDAB4D34}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3093,23 +3198,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92FEC7CF-4815-42BA-A053-9D2F9AB7FD60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD363066-8CBD-4D6F-8835-7EB8A1E12EC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="346a80a9-3278-4844-b436-58ae57568790"/>
-    <ds:schemaRef ds:uri="a2d094e0-efa8-4820-a0b3-29af30f3c512"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>